<commit_message>
Updated Budget to include current status as of 3/3/15
</commit_message>
<xml_diff>
--- a/EE_464K_Team_33_Partial_Budget_1-0.xlsx
+++ b/EE_464K_Team_33_Partial_Budget_1-0.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="9540"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="9540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Order List 2-9-15" sheetId="1" r:id="rId1"/>
+    <sheet name="Next Order List" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="56">
   <si>
     <t>LED Sockets</t>
   </si>
@@ -164,6 +165,24 @@
   </si>
   <si>
     <t>GroBot</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>X/X/2015</t>
+  </si>
+  <si>
+    <t>Digital Potentiometer ICs IC Dual 10-Bit SPI</t>
+  </si>
+  <si>
+    <t>Analog Devices</t>
+  </si>
+  <si>
+    <t>AD5235BRUZ250</t>
+  </si>
+  <si>
+    <t>584-AD5235BRUZ250</t>
   </si>
 </sst>
 </file>
@@ -695,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -751,21 +770,27 @@
       <c r="A6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="20" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1189,4 +1214,336 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="1">
+        <f>F13*G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="1">
+        <f t="shared" ref="H14:H17" si="0">F14*G14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="H18" s="22">
+        <f>SUM(H13:H17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="F19" s="3"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="F20" s="3"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="3">
+        <v>7.92</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22" s="1">
+        <f>F22*G22</f>
+        <v>15.84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="F23" s="3"/>
+      <c r="H23" s="1">
+        <f>F23*G23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="22">
+        <f>SUM(H22:H23)</f>
+        <v>15.84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="3"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="3"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="F31" s="3"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+      <c r="H32" s="22">
+        <f>SUM(H28:H31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>